<commit_message>
Ground human oversight moderator in automation theory (Parasuraman et al., 2000)
- Rewrite structured abstract (Computers & Education format) with theoretical
  grounding in established automation level taxonomy and EU AI Act (2024)
- Add Parasuraman et al. (2000), EU AI Act, Shneiderman (2022), Molenaar (2022),
  Holstein et al. (2019) references across all documents
- Update coding scheme, coding manual, and codebook with automation level
  mappings (Levels 7-10 → Autonomous, 4-6 → Checkpoints, 1-3 → Human-Led)
- Add pre-planned sensitivity analyses for oversight moderator cell imbalance
  (binary collapse, default-coded exclusion, confounding assessment) with R code
- Update Excel codebook (.xlsx) with cell comment on oversight taxonomy
- Update Word coding manual (.docx) with theoretical grounding paragraph
- Add decision D-07 to integration document decision log

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/templates/Agentic_AI_Learning_MA_Coding_v1.xlsx
+++ b/data/templates/Agentic_AI_Learning_MA_Coding_v1.xlsx
@@ -139,6 +139,27 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Meta-Analysis Coding Team</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <t>Human Oversight Level (Parasuraman et al., 2000)
+Three-level taxonomy grounded in the 10-level automation model:
+  fully_autonomous = Automation levels 7-10 (computer decides, may/may not inform human)
+  ai_led_checkpoints = Automation levels 4-6 (computer suggests/executes, human can intervene)
+  human_led_ai_support = Automation levels 1-3 (human decides with computer assistance)
+See coding_manual.md §C1 for full decision rules.
+Policy context: EU AI Act (2024, Art. 14) mandates human oversight for high-risk AI in education.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -543,6 +564,18 @@
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>[INSTRUCTIONS]</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Oversight taxonomy: Parasuraman et al. (2000) 10-level automation model collapsed to 3 levels. See AI_Agent_Characteristics sheet, column C.</t>
         </is>
       </c>
     </row>
@@ -883,6 +916,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 

</xml_diff>